<commit_message>
Kleine Fehlerbehebung DB; Mockup-Screenshots Update
</commit_message>
<xml_diff>
--- a/documents/Anforderungsartefakte/Ziele.xlsx
+++ b/documents/Anforderungsartefakte/Ziele.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -587,7 +587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D34" activeCellId="1" sqref="I12:S24 D34"/>
     </sheetView>
   </sheetViews>
@@ -686,7 +686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q4" sqref="C4:Q33"/>
     </sheetView>
   </sheetViews>

</xml_diff>